<commit_message>
payoff calculations for italiandirect corrected
</commit_message>
<xml_diff>
--- a/Else/Expenditures for 2017.xlsx
+++ b/Else/Expenditures for 2017.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Cash</t>
   </si>
@@ -85,6 +85,51 @@
   </si>
   <si>
     <t>Corrections</t>
+  </si>
+  <si>
+    <t>Friday, end of the week</t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>\item 50 * 20 euro = 1 000 euro</t>
+  </si>
+  <si>
+    <t>\item 160 * 10 euro = 1 600 euro</t>
+  </si>
+  <si>
+    <t>\item 160 * 5 euro = 800 euro</t>
+  </si>
+  <si>
+    <t>\item 200 * 2 euro = 400 euro</t>
+  </si>
+  <si>
+    <t>\item 180 * 1 euro = 180 euro</t>
+  </si>
+  <si>
+    <t>\item 40 * 50 snt = 20 euro</t>
+  </si>
+  <si>
+    <t>250 * 1</t>
+  </si>
+  <si>
+    <t>50 kertaa kymmenen euroa</t>
+  </si>
+  <si>
+    <t>50 kertaa viisi euroa</t>
+  </si>
+  <si>
+    <t>100 kertaa 2 euroa</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Actual ( correction)</t>
+  </si>
+  <si>
+    <t>Needed:</t>
   </si>
 </sst>
 </file>
@@ -415,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,13 +555,31 @@
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3">
+        <f>SUM(E8:G8)</f>
+        <v>250</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>240</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <f>SUM(E9:G9)</f>
+        <v>381</v>
+      </c>
+      <c r="E9">
+        <v>356</v>
+      </c>
+      <c r="F9">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -524,7 +587,7 @@
       </c>
       <c r="C10">
         <f>C6-C8-C9</f>
-        <v>3366</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -534,13 +597,39 @@
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3">
+        <f>SUM(E12:G12)</f>
+        <v>479</v>
+      </c>
+      <c r="E12">
+        <v>332</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <f xml:space="preserve"> 8+4+2+2+4.5+8.5+7+5+14+10+9+6+10+5+3+4+5.5+4.5+11+2+3+7+2</f>
+        <v>137</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <f>SUM(E13:G13)</f>
+        <v>493</v>
+      </c>
+      <c r="E13">
+        <v>309.5</v>
+      </c>
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <f>59 + 53 + 41.5</f>
+        <v>153.5</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
@@ -548,15 +637,18 @@
       </c>
       <c r="C14">
         <f>C10-C12-C13</f>
-        <v>3366</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43087</v>
       </c>
@@ -565,22 +657,22 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19">
         <f>C14-C17-C18</f>
-        <v>3366</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43088</v>
       </c>
@@ -589,25 +681,25 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23">
         <f>C19-C21-C22</f>
-        <v>3366</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -615,6 +707,136 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30">
+        <f>A30*B30</f>
+        <v>520</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>58</v>
+      </c>
+      <c r="C31">
+        <f>A31*B31</f>
+        <v>580</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31">
+        <f>50*10</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>65</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:C35" si="0">A32*B32</f>
+        <v>325</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32">
+        <f>50*5</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>63</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>197</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>197</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>0.5</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <f>SUM(C30:C35)</f>
+        <v>1766</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>